<commit_message>
NKGA2-positive natural killer cell remapped
Remap "NKGA2-positive natural killer cell"  as "natural killer cell" with NKGA2 in "extra" field.
</commit_message>
<xml_diff>
--- a/source_data/cell_type_frequency-response_components_mapping.xlsx
+++ b/source_data/cell_type_frequency-response_components_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth\Documents\GitHub\hipc-dashboard-pipeline\source_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E778D9-43AA-434D-B048-2C8CB0071BC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A01AE4-BC9D-460C-A528-4BE690D8D0C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HIPC_Dashboard-Cell_type_Freque" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="457">
   <si>
     <t>original_annotation</t>
   </si>
@@ -634,12 +634,6 @@
     <t>NK cells (CD14-/CD20-/CD3-/NK/NKG2A+)</t>
   </si>
   <si>
-    <t>NKGA2-positive natural killer cell</t>
-  </si>
-  <si>
-    <t>CL_0002439</t>
-  </si>
-  <si>
     <t>NK cells (CD14-/CD20-/CD3-/NK/NKP46+)</t>
   </si>
   <si>
@@ -1394,6 +1388,9 @@
   </si>
   <si>
     <t>PR_000001017, PR_000001203</t>
+  </si>
+  <si>
+    <t>NKGA2+</t>
   </si>
 </sst>
 </file>
@@ -2075,9 +2072,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA917"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B168" sqref="B168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2137,7 +2134,7 @@
     </row>
     <row r="2" spans="1:27">
       <c r="A2" s="36" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B2" s="37" t="s">
         <v>11</v>
@@ -2207,7 +2204,7 @@
     </row>
     <row r="4" spans="1:27">
       <c r="A4" s="24" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B4" s="37" t="s">
         <v>17</v>
@@ -2216,10 +2213,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="12"/>
@@ -2246,7 +2243,7 @@
     </row>
     <row r="5" spans="1:27">
       <c r="A5" s="25" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B5" s="37" t="s">
         <v>17</v>
@@ -2255,10 +2252,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F5" s="18"/>
       <c r="G5" s="31"/>
@@ -2285,7 +2282,7 @@
     </row>
     <row r="6" spans="1:27">
       <c r="A6" s="25" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B6" s="37" t="s">
         <v>17</v>
@@ -2294,10 +2291,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F6" s="18"/>
       <c r="G6" s="30"/>
@@ -2324,7 +2321,7 @@
     </row>
     <row r="7" spans="1:27">
       <c r="A7" s="26" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B7" s="37" t="s">
         <v>17</v>
@@ -2333,10 +2330,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F7" s="38" t="s">
         <v>145</v>
@@ -2365,7 +2362,7 @@
     </row>
     <row r="8" spans="1:27">
       <c r="A8" s="36" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B8" s="37" t="s">
         <v>17</v>
@@ -2374,10 +2371,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
@@ -2413,10 +2410,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="62" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E9" s="62" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F9" s="18"/>
       <c r="G9" s="30" t="s">
@@ -2454,13 +2451,13 @@
         <v>18</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F10" s="62" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="G10" s="62"/>
       <c r="H10" s="8"/>
@@ -2486,7 +2483,7 @@
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1">
       <c r="A11" s="24" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B11" s="37" t="s">
         <v>17</v>
@@ -2495,10 +2492,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="14" t="s">
@@ -2562,13 +2559,13 @@
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1">
       <c r="A13" s="51" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>28</v>
@@ -2601,7 +2598,7 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1">
       <c r="A14" s="36" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B14" s="37" t="s">
         <v>52</v>
@@ -2610,10 +2607,10 @@
         <v>53</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E14" s="38" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
@@ -2640,7 +2637,7 @@
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1">
       <c r="A15" s="50" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B15" s="37" t="s">
         <v>45</v>
@@ -2679,7 +2676,7 @@
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1">
       <c r="A16" s="24" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B16" s="37" t="s">
         <v>45</v>
@@ -2718,7 +2715,7 @@
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1">
       <c r="A17" s="37" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B17" s="37" t="s">
         <v>45</v>
@@ -2759,7 +2756,7 @@
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1">
       <c r="A18" s="50" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B18" s="37" t="s">
         <v>45</v>
@@ -2796,7 +2793,7 @@
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1">
       <c r="A19" s="36" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B19" s="37" t="s">
         <v>45</v>
@@ -2807,7 +2804,7 @@
       <c r="D19" s="18"/>
       <c r="E19" s="7"/>
       <c r="F19" s="63" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="8"/>
@@ -2868,7 +2865,7 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1">
       <c r="A21" s="32" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B21" s="37" t="s">
         <v>45</v>
@@ -2903,7 +2900,7 @@
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1">
       <c r="A22" s="43" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B22" s="37" t="s">
         <v>43</v>
@@ -2938,7 +2935,7 @@
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1">
       <c r="A23" s="42" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B23" s="37" t="s">
         <v>43</v>
@@ -2973,7 +2970,7 @@
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1">
       <c r="A24" s="23" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B24" s="37" t="s">
         <v>50</v>
@@ -3010,7 +3007,7 @@
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1">
       <c r="A25" s="36" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B25" s="37" t="s">
         <v>50</v>
@@ -3047,7 +3044,7 @@
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1">
       <c r="A26" s="23" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B26" s="37" t="s">
         <v>50</v>
@@ -3082,10 +3079,10 @@
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1">
       <c r="A27" s="51" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C27" s="41" t="s">
         <v>54</v>
@@ -3121,10 +3118,10 @@
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1">
       <c r="A28" s="36" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C28" s="41" t="s">
         <v>54</v>
@@ -3160,10 +3157,10 @@
     </row>
     <row r="29" spans="1:27" ht="15.75" customHeight="1">
       <c r="A29" s="60" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C29" s="41" t="s">
         <v>54</v>
@@ -3195,10 +3192,10 @@
     </row>
     <row r="30" spans="1:27" ht="15.75" customHeight="1">
       <c r="A30" s="51" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C30" s="41" t="s">
         <v>54</v>
@@ -3230,7 +3227,7 @@
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1">
       <c r="A31" s="36" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B31" s="37" t="s">
         <v>179</v>
@@ -3239,14 +3236,14 @@
         <v>180</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E31" s="38" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F31" s="18"/>
       <c r="G31" s="38" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
@@ -3271,7 +3268,7 @@
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
       <c r="A32" s="51" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B32" s="37" t="s">
         <v>179</v>
@@ -3283,7 +3280,7 @@
         <v>181</v>
       </c>
       <c r="E32" s="38" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F32" s="9" t="s">
         <v>119</v>
@@ -3349,7 +3346,7 @@
     </row>
     <row r="34" spans="1:27" ht="15.75" customHeight="1">
       <c r="A34" s="25" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B34" s="37" t="s">
         <v>33</v>
@@ -3358,10 +3355,10 @@
         <v>34</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
@@ -3388,7 +3385,7 @@
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1">
       <c r="A35" s="36" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B35" s="37" t="s">
         <v>33</v>
@@ -3466,7 +3463,7 @@
     </row>
     <row r="37" spans="1:27" ht="22.5" customHeight="1">
       <c r="A37" s="26" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B37" s="37" t="s">
         <v>33</v>
@@ -3475,13 +3472,13 @@
         <v>34</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E37" s="38" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G37" s="18"/>
       <c r="H37" s="9"/>
@@ -3507,7 +3504,7 @@
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1">
       <c r="A38" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B38" s="37" t="s">
         <v>33</v>
@@ -3516,13 +3513,13 @@
         <v>34</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E38" s="38" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F38" s="30" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G38" s="18"/>
       <c r="H38" s="8"/>
@@ -3548,7 +3545,7 @@
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
       <c r="A39" s="26" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B39" s="37" t="s">
         <v>33</v>
@@ -3557,10 +3554,10 @@
         <v>34</v>
       </c>
       <c r="D39" s="49" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E39" s="49" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F39" s="18"/>
       <c r="G39" s="29"/>
@@ -3587,7 +3584,7 @@
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
       <c r="A40" s="12" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B40" s="37" t="s">
         <v>33</v>
@@ -3596,10 +3593,10 @@
         <v>34</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E40" s="38" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F40" s="18"/>
       <c r="G40" s="18"/>
@@ -3667,7 +3664,7 @@
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1">
       <c r="A42" s="24" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B42" s="37" t="s">
         <v>33</v>
@@ -3747,7 +3744,7 @@
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1">
       <c r="A44" s="25" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B44" s="37" t="s">
         <v>33</v>
@@ -3756,10 +3753,10 @@
         <v>34</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
@@ -3786,7 +3783,7 @@
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1">
       <c r="A45" s="36" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B45" s="37" t="s">
         <v>33</v>
@@ -3825,7 +3822,7 @@
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1">
       <c r="A46" s="36" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B46" s="37" t="s">
         <v>33</v>
@@ -3834,13 +3831,13 @@
         <v>34</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E46" s="38" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F46" s="38" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="G46" s="10"/>
       <c r="H46" s="8"/>
@@ -3866,7 +3863,7 @@
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1">
       <c r="A47" s="50" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B47" s="37" t="s">
         <v>33</v>
@@ -3875,10 +3872,10 @@
         <v>34</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
@@ -3905,7 +3902,7 @@
     </row>
     <row r="48" spans="1:27" ht="15.75" customHeight="1">
       <c r="A48" s="26" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B48" s="37" t="s">
         <v>33</v>
@@ -3946,7 +3943,7 @@
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1">
       <c r="A49" s="26" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B49" s="37" t="s">
         <v>33</v>
@@ -3985,7 +3982,7 @@
     </row>
     <row r="50" spans="1:27" ht="15.75" customHeight="1">
       <c r="A50" s="50" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B50" s="37" t="s">
         <v>33</v>
@@ -3994,7 +3991,7 @@
         <v>34</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>165</v>
@@ -4063,7 +4060,7 @@
     </row>
     <row r="52" spans="1:27" ht="15.75" customHeight="1">
       <c r="A52" s="36" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B52" s="37" t="s">
         <v>33</v>
@@ -4072,14 +4069,14 @@
         <v>34</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E52" s="38" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F52" s="30"/>
       <c r="G52" s="63" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="H52" s="9"/>
       <c r="I52" s="9"/>
@@ -4143,7 +4140,7 @@
     </row>
     <row r="54" spans="1:27" ht="15.75" customHeight="1">
       <c r="A54" s="51" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B54" s="37" t="s">
         <v>33</v>
@@ -4152,10 +4149,10 @@
         <v>34</v>
       </c>
       <c r="D54" s="38" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E54" s="38" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F54" s="18"/>
       <c r="G54" s="18"/>
@@ -4182,7 +4179,7 @@
     </row>
     <row r="55" spans="1:27" ht="15.75" customHeight="1">
       <c r="A55" s="36" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B55" s="37" t="s">
         <v>33</v>
@@ -4193,7 +4190,7 @@
       <c r="D55" s="38"/>
       <c r="E55" s="18"/>
       <c r="F55" s="18" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G55" s="18"/>
       <c r="H55" s="8"/>
@@ -4256,7 +4253,7 @@
     </row>
     <row r="57" spans="1:27" ht="15.75" customHeight="1">
       <c r="A57" s="24" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B57" s="37" t="s">
         <v>33</v>
@@ -4293,7 +4290,7 @@
     </row>
     <row r="58" spans="1:27" ht="15.75" customHeight="1">
       <c r="A58" s="12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B58" s="37" t="s">
         <v>33</v>
@@ -4304,7 +4301,7 @@
       <c r="D58" s="18"/>
       <c r="E58" s="18"/>
       <c r="F58" s="18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G58" s="31"/>
       <c r="H58" s="8"/>
@@ -4365,7 +4362,7 @@
     </row>
     <row r="60" spans="1:27" ht="15.75" customHeight="1">
       <c r="A60" s="57" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B60" s="37" t="s">
         <v>33</v>
@@ -4400,7 +4397,7 @@
     </row>
     <row r="61" spans="1:27" ht="15.75" customHeight="1">
       <c r="A61" s="12" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B61" s="37" t="s">
         <v>33</v>
@@ -4435,7 +4432,7 @@
     </row>
     <row r="62" spans="1:27" ht="15.75" customHeight="1">
       <c r="A62" s="51" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B62" s="37" t="s">
         <v>81</v>
@@ -4444,10 +4441,10 @@
         <v>82</v>
       </c>
       <c r="D62" s="38" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="F62" s="30"/>
       <c r="G62" s="29"/>
@@ -4509,7 +4506,7 @@
     </row>
     <row r="64" spans="1:27" ht="15.75" customHeight="1">
       <c r="A64" s="36" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B64" s="37" t="s">
         <v>81</v>
@@ -4544,7 +4541,7 @@
     </row>
     <row r="65" spans="1:27" ht="15.75" customHeight="1">
       <c r="A65" s="50" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B65" s="37" t="s">
         <v>115</v>
@@ -4585,7 +4582,7 @@
     </row>
     <row r="66" spans="1:27" ht="15.75" customHeight="1">
       <c r="A66" s="25" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B66" s="37" t="s">
         <v>38</v>
@@ -4594,10 +4591,10 @@
         <v>39</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F66" s="9"/>
       <c r="G66" s="9"/>
@@ -4663,7 +4660,7 @@
     </row>
     <row r="68" spans="1:27" ht="15.75" customHeight="1">
       <c r="A68" s="12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B68" s="37" t="s">
         <v>38</v>
@@ -4672,10 +4669,10 @@
         <v>39</v>
       </c>
       <c r="D68" s="38" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E68" s="38" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F68" s="18"/>
       <c r="G68" s="18"/>
@@ -4702,7 +4699,7 @@
     </row>
     <row r="69" spans="1:27" ht="15.75" customHeight="1">
       <c r="A69" s="26" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B69" s="37" t="s">
         <v>38</v>
@@ -4711,10 +4708,10 @@
         <v>39</v>
       </c>
       <c r="D69" s="38" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E69" s="38" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F69" s="18"/>
       <c r="G69" s="30"/>
@@ -4780,7 +4777,7 @@
     </row>
     <row r="71" spans="1:27" ht="15.75" customHeight="1">
       <c r="A71" s="54" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B71" s="37" t="s">
         <v>38</v>
@@ -4858,7 +4855,7 @@
     </row>
     <row r="73" spans="1:27" ht="15.75" customHeight="1">
       <c r="A73" s="25" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B73" s="37" t="s">
         <v>38</v>
@@ -4867,10 +4864,10 @@
         <v>39</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
@@ -4897,7 +4894,7 @@
     </row>
     <row r="74" spans="1:27" ht="15.75" customHeight="1">
       <c r="A74" s="24" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B74" s="37" t="s">
         <v>38</v>
@@ -4912,7 +4909,7 @@
         <v>31</v>
       </c>
       <c r="F74" s="29" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G74" s="29"/>
       <c r="H74" s="8"/>
@@ -4977,7 +4974,7 @@
     </row>
     <row r="76" spans="1:27" ht="15.75" customHeight="1">
       <c r="A76" s="54" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B76" s="37" t="s">
         <v>38</v>
@@ -5016,7 +5013,7 @@
     </row>
     <row r="77" spans="1:27" ht="15.75" customHeight="1">
       <c r="A77" s="24" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B77" s="37" t="s">
         <v>38</v>
@@ -5025,10 +5022,10 @@
         <v>39</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E77" s="18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F77" s="9" t="s">
         <v>119</v>
@@ -5057,7 +5054,7 @@
     </row>
     <row r="78" spans="1:27" ht="15.75" customHeight="1">
       <c r="A78" s="50" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B78" s="37" t="s">
         <v>38</v>
@@ -5066,10 +5063,10 @@
         <v>39</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
@@ -5096,7 +5093,7 @@
     </row>
     <row r="79" spans="1:27" ht="15.75" customHeight="1">
       <c r="A79" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B79" s="37" t="s">
         <v>38</v>
@@ -5105,13 +5102,13 @@
         <v>39</v>
       </c>
       <c r="D79" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="F79" s="7" t="s">
         <v>217</v>
-      </c>
-      <c r="E79" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>219</v>
       </c>
       <c r="G79" s="10"/>
       <c r="H79" s="8"/>
@@ -5137,7 +5134,7 @@
     </row>
     <row r="80" spans="1:27" ht="15.75" customHeight="1">
       <c r="A80" s="9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B80" s="37" t="s">
         <v>38</v>
@@ -5146,13 +5143,13 @@
         <v>39</v>
       </c>
       <c r="D80" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="F80" s="9" t="s">
         <v>217</v>
-      </c>
-      <c r="E80" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="F80" s="9" t="s">
-        <v>219</v>
       </c>
       <c r="G80" s="9"/>
       <c r="H80" s="9"/>
@@ -5178,7 +5175,7 @@
     </row>
     <row r="81" spans="1:27" ht="15.75" customHeight="1">
       <c r="A81" s="36" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B81" s="37" t="s">
         <v>38</v>
@@ -5193,7 +5190,7 @@
         <v>136</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G81" s="10"/>
       <c r="H81" s="8"/>
@@ -5219,7 +5216,7 @@
     </row>
     <row r="82" spans="1:27" ht="15.75" customHeight="1">
       <c r="A82" s="50" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B82" s="37" t="s">
         <v>38</v>
@@ -5258,7 +5255,7 @@
     </row>
     <row r="83" spans="1:27" ht="15.75" customHeight="1">
       <c r="A83" s="12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B83" s="37" t="s">
         <v>38</v>
@@ -5267,10 +5264,10 @@
         <v>39</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E83" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F83" s="12"/>
       <c r="G83" s="9"/>
@@ -5297,7 +5294,7 @@
     </row>
     <row r="84" spans="1:27" ht="15.75" customHeight="1">
       <c r="A84" s="36" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B84" s="37" t="s">
         <v>38</v>
@@ -5308,7 +5305,7 @@
       <c r="D84" s="18"/>
       <c r="E84" s="7"/>
       <c r="F84" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G84" s="10"/>
       <c r="H84" s="8"/>
@@ -5334,7 +5331,7 @@
     </row>
     <row r="85" spans="1:27" ht="19.5" customHeight="1">
       <c r="A85" s="26" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B85" s="37" t="s">
         <v>38</v>
@@ -5345,7 +5342,7 @@
       <c r="D85" s="9"/>
       <c r="E85" s="9"/>
       <c r="F85" s="9" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G85" s="9"/>
       <c r="H85" s="8"/>
@@ -5408,7 +5405,7 @@
     </row>
     <row r="87" spans="1:27" ht="15.75" customHeight="1">
       <c r="A87" s="59" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B87" s="37" t="s">
         <v>38</v>
@@ -5445,7 +5442,7 @@
     </row>
     <row r="88" spans="1:27" ht="15.75" customHeight="1">
       <c r="A88" s="56" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B88" s="37" t="s">
         <v>38</v>
@@ -5480,7 +5477,7 @@
     </row>
     <row r="89" spans="1:27" ht="21" customHeight="1">
       <c r="A89" s="61" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B89" s="37" t="s">
         <v>38</v>
@@ -5515,7 +5512,7 @@
     </row>
     <row r="90" spans="1:27" ht="15.75" customHeight="1">
       <c r="A90" s="26" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B90" s="37" t="s">
         <v>38</v>
@@ -5585,7 +5582,7 @@
     </row>
     <row r="92" spans="1:27" ht="15.75" customHeight="1">
       <c r="A92" s="40" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B92" s="37" t="s">
         <v>61</v>
@@ -5655,7 +5652,7 @@
     </row>
     <row r="94" spans="1:27" ht="15.75" customHeight="1">
       <c r="A94" s="53" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B94" s="37" t="s">
         <v>97</v>
@@ -5690,7 +5687,7 @@
     </row>
     <row r="95" spans="1:27" ht="15.75" customHeight="1">
       <c r="A95" s="55" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B95" s="37" t="s">
         <v>113</v>
@@ -5699,10 +5696,10 @@
         <v>114</v>
       </c>
       <c r="D95" s="38" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E95" s="38" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="F95" s="30"/>
       <c r="G95" s="31"/>
@@ -5764,23 +5761,23 @@
     </row>
     <row r="97" spans="1:27" ht="15.75" customHeight="1">
       <c r="A97" s="36" t="s">
+        <v>349</v>
+      </c>
+      <c r="B97" s="37" t="s">
+        <v>350</v>
+      </c>
+      <c r="C97" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="D97" s="38" t="s">
         <v>351</v>
       </c>
-      <c r="B97" s="37" t="s">
-        <v>352</v>
-      </c>
-      <c r="C97" s="19" t="s">
-        <v>453</v>
-      </c>
-      <c r="D97" s="38" t="s">
-        <v>353</v>
-      </c>
       <c r="E97" s="38" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="F97" s="18"/>
       <c r="G97" s="63" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H97" s="9"/>
       <c r="I97" s="9"/>
@@ -5848,7 +5845,7 @@
     </row>
     <row r="99" spans="1:27" ht="15.75" customHeight="1">
       <c r="A99" s="26" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B99" s="37" t="s">
         <v>13</v>
@@ -6152,7 +6149,7 @@
     </row>
     <row r="107" spans="1:27" ht="15.75" customHeight="1">
       <c r="A107" s="16" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B107" s="37" t="s">
         <v>129</v>
@@ -6191,7 +6188,7 @@
     </row>
     <row r="108" spans="1:27" ht="15.75" customHeight="1">
       <c r="A108" s="16" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B108" s="37" t="s">
         <v>129</v>
@@ -6339,7 +6336,7 @@
     </row>
     <row r="112" spans="1:27" ht="15.75" customHeight="1">
       <c r="A112" s="36" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B112" s="37" t="s">
         <v>22</v>
@@ -6348,10 +6345,10 @@
         <v>23</v>
       </c>
       <c r="D112" s="38" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E112" s="38" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F112" s="18"/>
       <c r="G112" s="18"/>
@@ -6378,7 +6375,7 @@
     </row>
     <row r="113" spans="1:27" ht="15.75" customHeight="1">
       <c r="A113" s="50" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B113" s="37" t="s">
         <v>22</v>
@@ -6495,22 +6492,22 @@
     </row>
     <row r="116" spans="1:27" ht="15.75" customHeight="1">
       <c r="A116" s="36" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B116" s="37" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C116" s="41" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D116" s="38" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E116" s="38" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F116" s="29" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="G116" s="29"/>
       <c r="H116" s="8"/>
@@ -6536,22 +6533,22 @@
     </row>
     <row r="117" spans="1:27" ht="15.75" customHeight="1">
       <c r="A117" s="36" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B117" s="37" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C117" s="41" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D117" s="38" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E117" s="38" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F117" s="29" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="G117" s="37"/>
       <c r="H117" s="8"/>
@@ -6626,7 +6623,7 @@
       <c r="E119" s="18"/>
       <c r="F119" s="18"/>
       <c r="G119" s="29" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="H119" s="9"/>
       <c r="I119" s="9"/>
@@ -6660,10 +6657,10 @@
         <v>26</v>
       </c>
       <c r="D120" s="18" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E120" s="38" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F120" s="18"/>
       <c r="G120" s="30"/>
@@ -6727,7 +6724,7 @@
     </row>
     <row r="122" spans="1:27" ht="15.75" customHeight="1">
       <c r="A122" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B122" s="37" t="s">
         <v>174</v>
@@ -6797,7 +6794,7 @@
     </row>
     <row r="124" spans="1:27" ht="15.75" customHeight="1">
       <c r="A124" s="50" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B124" s="37" t="s">
         <v>73</v>
@@ -6873,7 +6870,7 @@
     </row>
     <row r="126" spans="1:27" ht="15.75" customHeight="1">
       <c r="A126" s="34" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B126" s="37" t="s">
         <v>85</v>
@@ -6882,13 +6879,13 @@
         <v>86</v>
       </c>
       <c r="D126" s="64" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E126" s="18" t="s">
         <v>93</v>
       </c>
       <c r="F126" s="18" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G126" s="29"/>
       <c r="H126" s="8"/>
@@ -6914,7 +6911,7 @@
     </row>
     <row r="127" spans="1:27" ht="15.75" customHeight="1">
       <c r="A127" s="33" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B127" s="37" t="s">
         <v>85</v>
@@ -6923,10 +6920,10 @@
         <v>86</v>
       </c>
       <c r="D127" s="18" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E127" s="18" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F127" s="18"/>
       <c r="G127" s="18"/>
@@ -7031,7 +7028,7 @@
     </row>
     <row r="130" spans="1:27" ht="15.75" customHeight="1">
       <c r="A130" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B130" s="37" t="s">
         <v>85</v>
@@ -7070,7 +7067,7 @@
     </row>
     <row r="131" spans="1:27" ht="15.75" customHeight="1">
       <c r="A131" s="23" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B131" s="37" t="s">
         <v>85</v>
@@ -7079,13 +7076,13 @@
         <v>86</v>
       </c>
       <c r="D131" s="18" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E131" s="21" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F131" s="7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G131" s="29"/>
       <c r="H131" s="8"/>
@@ -7111,7 +7108,7 @@
     </row>
     <row r="132" spans="1:27" ht="15.75" customHeight="1">
       <c r="A132" s="23" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B132" s="37" t="s">
         <v>85</v>
@@ -7120,13 +7117,13 @@
         <v>86</v>
       </c>
       <c r="D132" s="18" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E132" s="21" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F132" s="7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G132" s="29"/>
       <c r="H132" s="8"/>
@@ -7187,7 +7184,7 @@
     </row>
     <row r="134" spans="1:27" ht="15.75" customHeight="1">
       <c r="A134" s="16" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B134" s="37" t="s">
         <v>85</v>
@@ -7222,7 +7219,7 @@
     </row>
     <row r="135" spans="1:27" ht="15.75" customHeight="1">
       <c r="A135" s="33" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B135" s="37" t="s">
         <v>189</v>
@@ -7231,10 +7228,10 @@
         <v>190</v>
       </c>
       <c r="D135" s="38" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E135" s="10" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F135" s="7"/>
       <c r="G135" s="10"/>
@@ -7261,7 +7258,7 @@
     </row>
     <row r="136" spans="1:27" ht="15.75" customHeight="1">
       <c r="A136" s="23" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B136" s="37" t="s">
         <v>189</v>
@@ -7270,10 +7267,10 @@
         <v>190</v>
       </c>
       <c r="D136" s="18" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E136" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F136" s="18"/>
       <c r="G136" s="18"/>
@@ -7300,7 +7297,7 @@
     </row>
     <row r="137" spans="1:27" ht="15.75" customHeight="1">
       <c r="A137" s="33" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B137" s="37" t="s">
         <v>189</v>
@@ -7309,10 +7306,10 @@
         <v>190</v>
       </c>
       <c r="D137" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E137" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F137" s="7"/>
       <c r="G137" s="10"/>
@@ -7339,7 +7336,7 @@
     </row>
     <row r="138" spans="1:27" ht="18.75" customHeight="1">
       <c r="A138" s="47" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B138" s="37" t="s">
         <v>111</v>
@@ -7348,10 +7345,10 @@
         <v>112</v>
       </c>
       <c r="D138" s="38" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E138" s="38" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F138" s="38" t="s">
         <v>145</v>
@@ -7380,7 +7377,7 @@
     </row>
     <row r="139" spans="1:27" ht="15.75" customHeight="1">
       <c r="A139" s="36" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B139" s="37" t="s">
         <v>111</v>
@@ -7458,7 +7455,7 @@
     </row>
     <row r="141" spans="1:27" ht="15.75" customHeight="1">
       <c r="A141" s="25" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B141" s="37" t="s">
         <v>111</v>
@@ -7532,7 +7529,7 @@
     </row>
     <row r="143" spans="1:27" ht="15.75" customHeight="1">
       <c r="A143" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B143" s="37" t="s">
         <v>7</v>
@@ -7544,7 +7541,7 @@
         <v>197</v>
       </c>
       <c r="E143" s="18" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F143" s="18" t="s">
         <v>198</v>
@@ -7582,10 +7579,10 @@
         <v>8</v>
       </c>
       <c r="D144" s="44" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E144" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F144" s="7" t="s">
         <v>198</v>
@@ -7614,7 +7611,7 @@
     </row>
     <row r="145" spans="1:27" ht="15.75" customHeight="1">
       <c r="A145" s="48" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B145" s="37" t="s">
         <v>7</v>
@@ -7623,10 +7620,10 @@
         <v>8</v>
       </c>
       <c r="D145" s="46" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E145" s="38" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="F145" s="7" t="s">
         <v>198</v>
@@ -7664,10 +7661,10 @@
         <v>8</v>
       </c>
       <c r="D146" s="46" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E146" s="46" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F146" s="7" t="s">
         <v>198</v>
@@ -7705,10 +7702,10 @@
         <v>8</v>
       </c>
       <c r="D147" s="18" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E147" s="18" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F147" s="18"/>
       <c r="G147" s="18"/>
@@ -7735,7 +7732,7 @@
     </row>
     <row r="148" spans="1:27" ht="15.75" customHeight="1">
       <c r="A148" s="9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B148" s="37" t="s">
         <v>7</v>
@@ -7744,10 +7741,10 @@
         <v>8</v>
       </c>
       <c r="D148" s="10" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E148" s="10" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F148" s="7"/>
       <c r="G148" s="10"/>
@@ -7774,7 +7771,7 @@
     </row>
     <row r="149" spans="1:27" ht="15.75" customHeight="1">
       <c r="A149" s="36" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B149" s="37" t="s">
         <v>7</v>
@@ -7783,10 +7780,10 @@
         <v>8</v>
       </c>
       <c r="D149" s="29" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E149" s="29" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F149" s="7"/>
       <c r="G149" s="29"/>
@@ -7813,7 +7810,7 @@
     </row>
     <row r="150" spans="1:27" ht="15.75" customHeight="1">
       <c r="A150" s="25" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B150" s="37" t="s">
         <v>7</v>
@@ -7822,10 +7819,10 @@
         <v>8</v>
       </c>
       <c r="D150" s="29" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E150" s="9" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F150" s="9"/>
       <c r="G150" s="29"/>
@@ -7852,7 +7849,7 @@
     </row>
     <row r="151" spans="1:27" ht="15.75" customHeight="1">
       <c r="A151" s="33" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B151" s="37" t="s">
         <v>7</v>
@@ -7861,10 +7858,10 @@
         <v>8</v>
       </c>
       <c r="D151" s="18" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E151" s="18" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F151" s="7"/>
       <c r="G151" s="10"/>
@@ -7891,7 +7888,7 @@
     </row>
     <row r="152" spans="1:27" ht="15.75" customHeight="1">
       <c r="A152" s="23" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B152" s="37" t="s">
         <v>7</v>
@@ -7900,10 +7897,10 @@
         <v>8</v>
       </c>
       <c r="D152" s="30" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E152" s="30" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F152" s="7"/>
       <c r="G152" s="30"/>
@@ -7930,7 +7927,7 @@
     </row>
     <row r="153" spans="1:27" ht="15.75" customHeight="1">
       <c r="A153" s="35" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B153" s="37" t="s">
         <v>7</v>
@@ -7939,7 +7936,7 @@
         <v>8</v>
       </c>
       <c r="D153" s="15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E153" s="15" t="s">
         <v>10</v>
@@ -8008,7 +8005,7 @@
     </row>
     <row r="155" spans="1:27" ht="21" customHeight="1">
       <c r="A155" s="23" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B155" s="37" t="s">
         <v>7</v>
@@ -8047,7 +8044,7 @@
     </row>
     <row r="156" spans="1:27" ht="15.75" customHeight="1">
       <c r="A156" s="23" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B156" s="37" t="s">
         <v>7</v>
@@ -8086,7 +8083,7 @@
     </row>
     <row r="157" spans="1:27" ht="15.75" customHeight="1">
       <c r="A157" s="23" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B157" s="37" t="s">
         <v>7</v>
@@ -8125,7 +8122,7 @@
     </row>
     <row r="158" spans="1:27" ht="15.75" customHeight="1">
       <c r="A158" s="20" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B158" s="37" t="s">
         <v>7</v>
@@ -8134,7 +8131,7 @@
         <v>8</v>
       </c>
       <c r="D158" s="18" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E158" s="18" t="s">
         <v>91</v>
@@ -8164,7 +8161,7 @@
     </row>
     <row r="159" spans="1:27" ht="15.75" customHeight="1">
       <c r="A159" s="23" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B159" s="37" t="s">
         <v>7</v>
@@ -8173,7 +8170,7 @@
         <v>8</v>
       </c>
       <c r="D159" s="18" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E159" s="18" t="s">
         <v>91</v>
@@ -8203,7 +8200,7 @@
     </row>
     <row r="160" spans="1:27" ht="15.75" customHeight="1">
       <c r="A160" s="23" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B160" s="37" t="s">
         <v>7</v>
@@ -8212,7 +8209,7 @@
         <v>8</v>
       </c>
       <c r="D160" s="18" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E160" s="10" t="s">
         <v>91</v>
@@ -8242,7 +8239,7 @@
     </row>
     <row r="161" spans="1:27" ht="30.75" customHeight="1">
       <c r="A161" s="36" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B161" s="37" t="s">
         <v>7</v>
@@ -8251,16 +8248,16 @@
         <v>8</v>
       </c>
       <c r="D161" s="38" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E161" s="38" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F161" s="38" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G161" s="38" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="H161" s="8"/>
       <c r="I161" s="8"/>
@@ -8285,7 +8282,7 @@
     </row>
     <row r="162" spans="1:27" ht="15.75" customHeight="1">
       <c r="A162" s="34" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B162" s="37" t="s">
         <v>7</v>
@@ -8324,7 +8321,7 @@
     </row>
     <row r="163" spans="1:27" ht="15.75" customHeight="1">
       <c r="A163" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B163" s="37" t="s">
         <v>7</v>
@@ -8365,7 +8362,7 @@
     </row>
     <row r="164" spans="1:27" ht="15.75" customHeight="1">
       <c r="A164" s="34" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B164" s="68" t="s">
         <v>7</v>
@@ -8508,18 +8505,20 @@
         <v>203</v>
       </c>
       <c r="B168" s="37" t="s">
-        <v>204</v>
-      </c>
-      <c r="C168" s="41" t="s">
-        <v>205</v>
+        <v>7</v>
+      </c>
+      <c r="C168" s="67" t="s">
+        <v>8</v>
       </c>
       <c r="D168" s="38" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E168" s="38" t="s">
-        <v>429</v>
-      </c>
-      <c r="F168" s="7"/>
+        <v>427</v>
+      </c>
+      <c r="F168" s="7" t="s">
+        <v>456</v>
+      </c>
       <c r="G168" s="10"/>
       <c r="H168" s="8"/>
       <c r="I168" s="8"/>
@@ -8544,13 +8543,13 @@
     </row>
     <row r="169" spans="1:27" ht="15.75" customHeight="1">
       <c r="A169" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B169" s="37" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C169" s="41" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D169" s="18"/>
       <c r="E169" s="18"/>
@@ -8579,13 +8578,13 @@
     </row>
     <row r="170" spans="1:27" ht="15.75" customHeight="1">
       <c r="A170" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B170" s="37" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C170" s="41" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D170" s="18"/>
       <c r="E170" s="18"/>
@@ -8614,7 +8613,7 @@
     </row>
     <row r="171" spans="1:27" ht="15.75" customHeight="1">
       <c r="A171" s="36" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B171" s="37" t="s">
         <v>56</v>
@@ -8623,10 +8622,10 @@
         <v>57</v>
       </c>
       <c r="D171" s="38" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E171" s="38" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F171" s="7"/>
       <c r="G171" s="10"/>
@@ -8692,7 +8691,7 @@
     </row>
     <row r="173" spans="1:27" ht="15.75" customHeight="1">
       <c r="A173" s="40" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B173" s="37" t="s">
         <v>56</v>
@@ -8701,10 +8700,10 @@
         <v>57</v>
       </c>
       <c r="D173" s="38" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E173" s="38" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F173" s="7"/>
       <c r="G173" s="10"/>
@@ -8740,7 +8739,7 @@
         <v>57</v>
       </c>
       <c r="D174" s="18" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E174" s="38" t="s">
         <v>66</v>
@@ -8805,13 +8804,13 @@
     </row>
     <row r="176" spans="1:27" ht="15.75" customHeight="1">
       <c r="A176" s="36" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B176" s="37" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C176" s="41" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D176" s="38" t="s">
         <v>87</v>
@@ -8819,7 +8818,7 @@
       <c r="E176" s="18"/>
       <c r="F176" s="7"/>
       <c r="G176" s="38" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H176" s="8"/>
       <c r="I176" s="8"/>
@@ -8844,19 +8843,19 @@
     </row>
     <row r="177" spans="1:27" ht="15.75" customHeight="1">
       <c r="A177" s="33" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B177" s="37" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C177" s="41" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D177" s="29" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E177" s="18" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F177" s="18"/>
       <c r="G177" s="10"/>
@@ -8883,19 +8882,19 @@
     </row>
     <row r="178" spans="1:27" ht="15.75" customHeight="1">
       <c r="A178" s="36" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B178" s="37" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C178" s="41" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D178" s="62" t="s">
         <v>104</v>
       </c>
       <c r="E178" s="38" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F178" s="18"/>
       <c r="G178" s="18"/>
@@ -8922,13 +8921,13 @@
     </row>
     <row r="179" spans="1:27" ht="15.75" customHeight="1">
       <c r="A179" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B179" s="37" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C179" s="41" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D179" s="18"/>
       <c r="E179" s="18"/>
@@ -8957,19 +8956,19 @@
     </row>
     <row r="180" spans="1:27" ht="15.75" customHeight="1">
       <c r="A180" s="36" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B180" s="37" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C180" s="41" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D180" s="38" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E180" s="38" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F180" s="30"/>
       <c r="G180" s="30"/>
@@ -9035,7 +9034,7 @@
     </row>
     <row r="182" spans="1:27" ht="15.75" customHeight="1">
       <c r="A182" s="36" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B182" s="37" t="s">
         <v>172</v>
@@ -9074,7 +9073,7 @@
     </row>
     <row r="183" spans="1:27" ht="15.75" customHeight="1">
       <c r="A183" s="16" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B183" s="37" t="s">
         <v>172</v>
@@ -9109,19 +9108,19 @@
     </row>
     <row r="184" spans="1:27" ht="15.75" customHeight="1">
       <c r="A184" s="23" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B184" s="37" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C184" s="41" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D184" s="38" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E184" s="38" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F184" s="18"/>
       <c r="G184" s="10"/>
@@ -9148,13 +9147,13 @@
     </row>
     <row r="185" spans="1:27" ht="15.75" customHeight="1">
       <c r="A185" s="36" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B185" s="37" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C185" s="41" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D185" s="18" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
Read curation sheets in tsv instead of xlsx form.
Curation sheets will be saved from the master Google sheet directly to tsv files.  Associated code to deal with oddities of reading in Excel files removed.  cell type mapping updated to remove some em-dashes.
</commit_message>
<xml_diff>
--- a/source_data/cell_type_frequency-response_components_mapping.xlsx
+++ b/source_data/cell_type_frequency-response_components_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth\Documents\GitHub\hipc-dashboard-pipeline\source_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A01AE4-BC9D-460C-A528-4BE690D8D0C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117097A9-4C42-427B-A641-8B733BBF5440}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28455" yWindow="2925" windowWidth="30180" windowHeight="14475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HIPC_Dashboard-Cell_type_Freque" sheetId="1" r:id="rId1"/>
@@ -1120,9 +1120,6 @@
     <t>IFN-gamma+ antigen specific T cell</t>
   </si>
   <si>
-    <t>IgG+ memory B cells (CD3−, CD19+, HLADR+, CD27+, CD10−, CD20+, IgG+)</t>
-  </si>
-  <si>
     <t>IL22+ of CD161- CD4+ T cells</t>
   </si>
   <si>
@@ -1138,9 +1135,6 @@
     <t>plasmablasts (CD19+, CD27+, CD38+)</t>
   </si>
   <si>
-    <t>switched IgG+ memory B cells (CD3−, CD19+, HLADR+, CD27+, IgG+)</t>
-  </si>
-  <si>
     <t>T cells CD3+/CD4+/CD28+</t>
   </si>
   <si>
@@ -1391,6 +1385,12 @@
   </si>
   <si>
     <t>NKGA2+</t>
+  </si>
+  <si>
+    <t>switched IgG+ memory B cells (CD3-, CD19+, HLADR+, CD27+, IgG+)</t>
+  </si>
+  <si>
+    <t>IgG+ memory B cells (CD3-, CD19+, HLADR+, CD27+, CD10-, CD20+, IgG+)</t>
   </si>
 </sst>
 </file>
@@ -2073,8 +2073,8 @@
   <dimension ref="A1:AA917"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B168" sqref="B168"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2213,10 +2213,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="12"/>
@@ -2252,10 +2252,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F5" s="18"/>
       <c r="G5" s="31"/>
@@ -2291,10 +2291,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F6" s="18"/>
       <c r="G6" s="30"/>
@@ -2321,7 +2321,7 @@
     </row>
     <row r="7" spans="1:27">
       <c r="A7" s="26" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B7" s="37" t="s">
         <v>17</v>
@@ -2330,10 +2330,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="F7" s="38" t="s">
         <v>145</v>
@@ -2371,10 +2371,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
@@ -2410,10 +2410,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="62" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E9" s="62" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F9" s="18"/>
       <c r="G9" s="30" t="s">
@@ -2451,13 +2451,13 @@
         <v>18</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F10" s="62" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="G10" s="62"/>
       <c r="H10" s="8"/>
@@ -2492,10 +2492,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="14" t="s">
@@ -2565,7 +2565,7 @@
         <v>355</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>28</v>
@@ -2715,7 +2715,7 @@
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1">
       <c r="A17" s="37" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B17" s="37" t="s">
         <v>45</v>
@@ -2793,7 +2793,7 @@
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1">
       <c r="A19" s="36" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B19" s="37" t="s">
         <v>45</v>
@@ -2804,7 +2804,7 @@
       <c r="D19" s="18"/>
       <c r="E19" s="7"/>
       <c r="F19" s="63" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="8"/>
@@ -3268,7 +3268,7 @@
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
       <c r="A32" s="51" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B32" s="37" t="s">
         <v>179</v>
@@ -3280,7 +3280,7 @@
         <v>181</v>
       </c>
       <c r="E32" s="38" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F32" s="9" t="s">
         <v>119</v>
@@ -3472,10 +3472,10 @@
         <v>34</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E37" s="38" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F37" s="18" t="s">
         <v>221</v>
@@ -3513,10 +3513,10 @@
         <v>34</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E38" s="38" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F38" s="30" t="s">
         <v>223</v>
@@ -3545,7 +3545,7 @@
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
       <c r="A39" s="26" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B39" s="37" t="s">
         <v>33</v>
@@ -3554,10 +3554,10 @@
         <v>34</v>
       </c>
       <c r="D39" s="49" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E39" s="49" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F39" s="18"/>
       <c r="G39" s="29"/>
@@ -3593,10 +3593,10 @@
         <v>34</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E40" s="38" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F40" s="18"/>
       <c r="G40" s="18"/>
@@ -3822,7 +3822,7 @@
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1">
       <c r="A46" s="36" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B46" s="37" t="s">
         <v>33</v>
@@ -3837,7 +3837,7 @@
         <v>246</v>
       </c>
       <c r="F46" s="38" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G46" s="10"/>
       <c r="H46" s="8"/>
@@ -4060,7 +4060,7 @@
     </row>
     <row r="52" spans="1:27" ht="15.75" customHeight="1">
       <c r="A52" s="36" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B52" s="37" t="s">
         <v>33</v>
@@ -4069,14 +4069,14 @@
         <v>34</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E52" s="38" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F52" s="30"/>
       <c r="G52" s="63" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H52" s="9"/>
       <c r="I52" s="9"/>
@@ -4140,7 +4140,7 @@
     </row>
     <row r="54" spans="1:27" ht="15.75" customHeight="1">
       <c r="A54" s="51" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B54" s="37" t="s">
         <v>33</v>
@@ -4149,10 +4149,10 @@
         <v>34</v>
       </c>
       <c r="D54" s="38" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E54" s="38" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F54" s="18"/>
       <c r="G54" s="18"/>
@@ -4190,7 +4190,7 @@
       <c r="D55" s="38"/>
       <c r="E55" s="18"/>
       <c r="F55" s="18" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G55" s="18"/>
       <c r="H55" s="8"/>
@@ -4441,10 +4441,10 @@
         <v>82</v>
       </c>
       <c r="D62" s="38" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F62" s="30"/>
       <c r="G62" s="29"/>
@@ -4669,10 +4669,10 @@
         <v>39</v>
       </c>
       <c r="D68" s="38" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E68" s="38" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F68" s="18"/>
       <c r="G68" s="18"/>
@@ -4708,10 +4708,10 @@
         <v>39</v>
       </c>
       <c r="D69" s="38" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E69" s="38" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F69" s="18"/>
       <c r="G69" s="30"/>
@@ -5190,7 +5190,7 @@
         <v>136</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G81" s="10"/>
       <c r="H81" s="8"/>
@@ -5305,7 +5305,7 @@
       <c r="D84" s="18"/>
       <c r="E84" s="7"/>
       <c r="F84" s="7" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G84" s="10"/>
       <c r="H84" s="8"/>
@@ -5699,7 +5699,7 @@
         <v>351</v>
       </c>
       <c r="E95" s="38" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F95" s="30"/>
       <c r="G95" s="31"/>
@@ -5767,13 +5767,13 @@
         <v>350</v>
       </c>
       <c r="C97" s="19" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D97" s="38" t="s">
         <v>351</v>
       </c>
       <c r="E97" s="38" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F97" s="18"/>
       <c r="G97" s="63" t="s">
@@ -6336,7 +6336,7 @@
     </row>
     <row r="112" spans="1:27" ht="15.75" customHeight="1">
       <c r="A112" s="36" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B112" s="37" t="s">
         <v>22</v>
@@ -6345,10 +6345,10 @@
         <v>23</v>
       </c>
       <c r="D112" s="38" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E112" s="38" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F112" s="18"/>
       <c r="G112" s="18"/>
@@ -6375,7 +6375,7 @@
     </row>
     <row r="113" spans="1:27" ht="15.75" customHeight="1">
       <c r="A113" s="50" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B113" s="37" t="s">
         <v>22</v>
@@ -6492,22 +6492,22 @@
     </row>
     <row r="116" spans="1:27" ht="15.75" customHeight="1">
       <c r="A116" s="36" t="s">
-        <v>372</v>
+        <v>455</v>
       </c>
       <c r="B116" s="37" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C116" s="41" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D116" s="38" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E116" s="38" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F116" s="29" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G116" s="29"/>
       <c r="H116" s="8"/>
@@ -6533,22 +6533,22 @@
     </row>
     <row r="117" spans="1:27" ht="15.75" customHeight="1">
       <c r="A117" s="36" t="s">
-        <v>366</v>
+        <v>456</v>
       </c>
       <c r="B117" s="37" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C117" s="41" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D117" s="38" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E117" s="38" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="F117" s="29" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G117" s="37"/>
       <c r="H117" s="8"/>
@@ -6623,7 +6623,7 @@
       <c r="E119" s="18"/>
       <c r="F119" s="18"/>
       <c r="G119" s="29" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="H119" s="9"/>
       <c r="I119" s="9"/>
@@ -6657,10 +6657,10 @@
         <v>26</v>
       </c>
       <c r="D120" s="18" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E120" s="38" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F120" s="18"/>
       <c r="G120" s="30"/>
@@ -6794,7 +6794,7 @@
     </row>
     <row r="124" spans="1:27" ht="15.75" customHeight="1">
       <c r="A124" s="50" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B124" s="37" t="s">
         <v>73</v>
@@ -7231,7 +7231,7 @@
         <v>253</v>
       </c>
       <c r="E135" s="10" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="F135" s="7"/>
       <c r="G135" s="10"/>
@@ -7345,10 +7345,10 @@
         <v>112</v>
       </c>
       <c r="D138" s="38" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E138" s="38" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F138" s="38" t="s">
         <v>145</v>
@@ -7579,10 +7579,10 @@
         <v>8</v>
       </c>
       <c r="D144" s="44" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E144" s="38" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F144" s="7" t="s">
         <v>198</v>
@@ -7611,7 +7611,7 @@
     </row>
     <row r="145" spans="1:27" ht="15.75" customHeight="1">
       <c r="A145" s="48" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B145" s="37" t="s">
         <v>7</v>
@@ -7620,10 +7620,10 @@
         <v>8</v>
       </c>
       <c r="D145" s="46" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E145" s="38" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F145" s="7" t="s">
         <v>198</v>
@@ -7661,10 +7661,10 @@
         <v>8</v>
       </c>
       <c r="D146" s="46" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E146" s="46" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F146" s="7" t="s">
         <v>198</v>
@@ -7702,10 +7702,10 @@
         <v>8</v>
       </c>
       <c r="D147" s="18" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E147" s="18" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F147" s="18"/>
       <c r="G147" s="18"/>
@@ -7741,10 +7741,10 @@
         <v>8</v>
       </c>
       <c r="D148" s="10" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E148" s="10" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="F148" s="7"/>
       <c r="G148" s="10"/>
@@ -7780,10 +7780,10 @@
         <v>8</v>
       </c>
       <c r="D149" s="29" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E149" s="29" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F149" s="7"/>
       <c r="G149" s="29"/>
@@ -7819,10 +7819,10 @@
         <v>8</v>
       </c>
       <c r="D150" s="29" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E150" s="9" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F150" s="9"/>
       <c r="G150" s="29"/>
@@ -8239,7 +8239,7 @@
     </row>
     <row r="161" spans="1:27" ht="30.75" customHeight="1">
       <c r="A161" s="36" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B161" s="37" t="s">
         <v>7</v>
@@ -8251,13 +8251,13 @@
         <v>205</v>
       </c>
       <c r="E161" s="38" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F161" s="38" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="G161" s="38" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H161" s="8"/>
       <c r="I161" s="8"/>
@@ -8511,13 +8511,13 @@
         <v>8</v>
       </c>
       <c r="D168" s="38" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E168" s="38" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F168" s="7" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="G168" s="10"/>
       <c r="H168" s="8"/>
@@ -8578,7 +8578,7 @@
     </row>
     <row r="170" spans="1:27" ht="15.75" customHeight="1">
       <c r="A170" s="11" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B170" s="37" t="s">
         <v>210</v>
@@ -8613,7 +8613,7 @@
     </row>
     <row r="171" spans="1:27" ht="15.75" customHeight="1">
       <c r="A171" s="36" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B171" s="37" t="s">
         <v>56</v>
@@ -8622,10 +8622,10 @@
         <v>57</v>
       </c>
       <c r="D171" s="38" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E171" s="38" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F171" s="7"/>
       <c r="G171" s="10"/>
@@ -8739,7 +8739,7 @@
         <v>57</v>
       </c>
       <c r="D174" s="18" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E174" s="38" t="s">
         <v>66</v>
@@ -8894,7 +8894,7 @@
         <v>104</v>
       </c>
       <c r="E178" s="38" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F178" s="18"/>
       <c r="G178" s="18"/>
@@ -8956,7 +8956,7 @@
     </row>
     <row r="180" spans="1:27" ht="15.75" customHeight="1">
       <c r="A180" s="36" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B180" s="37" t="s">
         <v>241</v>
@@ -8965,10 +8965,10 @@
         <v>242</v>
       </c>
       <c r="D180" s="38" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E180" s="38" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F180" s="30"/>
       <c r="G180" s="30"/>
@@ -9117,10 +9117,10 @@
         <v>240</v>
       </c>
       <c r="D184" s="38" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E184" s="38" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F184" s="18"/>
       <c r="G184" s="10"/>

</xml_diff>

<commit_message>
change ontology separator character to match data
change "_" to ":"
</commit_message>
<xml_diff>
--- a/source_data/cell_type_frequency-response_components_mapping.xlsx
+++ b/source_data/cell_type_frequency-response_components_mapping.xlsx
@@ -654,9 +654,6 @@
     <t>monocytes</t>
   </si>
   <si>
-    <t>naive B cells (CD19-positive, IgD-negative, CD27-negative) (CL_0000788)</t>
-  </si>
-  <si>
     <t>TIV-specific CD8+ GRZ+ T lymphocyte cells</t>
   </si>
   <si>
@@ -729,9 +726,6 @@
     <t>triple-positive (interferon-gamma, tumor necrosis factor-alpha, interleukin-2) CD4 T cells</t>
   </si>
   <si>
-    <t>transitional B cells (CD19+, CD24+, CD38+) (CL_0000818)</t>
-  </si>
-  <si>
     <t>CD3- CD56dim Natural Killer cells</t>
   </si>
   <si>
@@ -969,9 +963,6 @@
     <t>IL22+ of CD161- CD4+ T cells</t>
   </si>
   <si>
-    <t>memory B cells (CD19+, IgD-, CD27+) (CL_0001053)</t>
-  </si>
-  <si>
     <t>memory T cells VZV-specific CD4+ IL2+ BCL2+</t>
   </si>
   <si>
@@ -1387,6 +1378,15 @@
   </si>
   <si>
     <t>PR:000001002, PR:000001932, PR:000001408</t>
+  </si>
+  <si>
+    <t>naive B cells (CD19-positive, IgD-negative, CD27-negative) (CL:0000788)</t>
+  </si>
+  <si>
+    <t>transitional B cells (CD19+, CD24+, CD38+) (CL:0000818)</t>
+  </si>
+  <si>
+    <t>memory B cells (CD19+, IgD-, CD27+) (CL:0001053)</t>
   </si>
 </sst>
 </file>
@@ -2069,8 +2069,8 @@
   <dimension ref="A1:AA917"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E184" sqref="E1:E1048576"/>
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2130,13 +2130,13 @@
     </row>
     <row r="2" spans="1:27">
       <c r="A2" s="36" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B2" s="37" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
@@ -2171,7 +2171,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
@@ -2200,19 +2200,19 @@
     </row>
     <row r="4" spans="1:27">
       <c r="A4" s="24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B4" s="37" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="12"/>
@@ -2239,19 +2239,19 @@
     </row>
     <row r="5" spans="1:27">
       <c r="A5" s="25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B5" s="37" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="F5" s="18"/>
       <c r="G5" s="31"/>
@@ -2278,19 +2278,19 @@
     </row>
     <row r="6" spans="1:27">
       <c r="A6" s="25" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B6" s="37" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="F6" s="18"/>
       <c r="G6" s="30"/>
@@ -2317,19 +2317,19 @@
     </row>
     <row r="7" spans="1:27">
       <c r="A7" s="26" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B7" s="37" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="F7" s="38" t="s">
         <v>114</v>
@@ -2358,19 +2358,19 @@
     </row>
     <row r="8" spans="1:27">
       <c r="A8" s="36" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B8" s="37" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
@@ -2403,13 +2403,13 @@
         <v>12</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D9" s="62" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E9" s="62" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="F9" s="18"/>
       <c r="G9" s="30" t="s">
@@ -2444,16 +2444,16 @@
         <v>12</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D10" s="29" t="s">
+        <v>361</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>427</v>
+      </c>
+      <c r="F10" s="62" t="s">
         <v>364</v>
-      </c>
-      <c r="E10" s="38" t="s">
-        <v>430</v>
-      </c>
-      <c r="F10" s="62" t="s">
-        <v>367</v>
       </c>
       <c r="G10" s="62"/>
       <c r="H10" s="8"/>
@@ -2479,19 +2479,19 @@
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1">
       <c r="A11" s="24" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B11" s="37" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="14" t="s">
@@ -2526,7 +2526,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
@@ -2555,13 +2555,13 @@
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1">
       <c r="A13" s="51" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>20</v>
@@ -2594,19 +2594,19 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1">
       <c r="A14" s="36" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B14" s="37" t="s">
         <v>39</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E14" s="38" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
@@ -2633,13 +2633,13 @@
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1">
       <c r="A15" s="50" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B15" s="37" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>144</v>
@@ -2672,13 +2672,13 @@
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1">
       <c r="A16" s="24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B16" s="37" t="s">
         <v>34</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>146</v>
@@ -2711,13 +2711,13 @@
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1">
       <c r="A17" s="37" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B17" s="37" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>35</v>
@@ -2752,13 +2752,13 @@
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1">
       <c r="A18" s="50" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B18" s="37" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>149</v>
@@ -2789,18 +2789,18 @@
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1">
       <c r="A19" s="36" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B19" s="37" t="s">
         <v>34</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="7"/>
       <c r="F19" s="63" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="8"/>
@@ -2832,7 +2832,7 @@
         <v>34</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D20" s="29"/>
       <c r="E20" s="29"/>
@@ -2861,13 +2861,13 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1">
       <c r="A21" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B21" s="37" t="s">
         <v>34</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D21" s="29"/>
       <c r="E21" s="29"/>
@@ -2896,13 +2896,13 @@
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1">
       <c r="A22" s="43" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B22" s="37" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
@@ -2931,13 +2931,13 @@
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1">
       <c r="A23" s="42" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B23" s="37" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
@@ -2966,13 +2966,13 @@
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1">
       <c r="A24" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B24" s="37" t="s">
         <v>38</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="18"/>
@@ -3003,13 +3003,13 @@
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1">
       <c r="A25" s="36" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B25" s="37" t="s">
         <v>38</v>
       </c>
       <c r="C25" s="41" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
@@ -3040,13 +3040,13 @@
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1">
       <c r="A26" s="23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B26" s="37" t="s">
         <v>38</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
@@ -3075,19 +3075,19 @@
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1">
       <c r="A27" s="51" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C27" s="41" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D27" s="38" t="s">
         <v>71</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="F27" s="30"/>
       <c r="G27" s="18"/>
@@ -3114,19 +3114,19 @@
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1">
       <c r="A28" s="36" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C28" s="41" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D28" s="38" t="s">
         <v>71</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="F28" s="18"/>
       <c r="G28" s="18"/>
@@ -3153,13 +3153,13 @@
     </row>
     <row r="29" spans="1:27" ht="15.75" customHeight="1">
       <c r="A29" s="60" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C29" s="41" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D29" s="39"/>
       <c r="E29" s="15"/>
@@ -3188,13 +3188,13 @@
     </row>
     <row r="30" spans="1:27" ht="15.75" customHeight="1">
       <c r="A30" s="51" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C30" s="41" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D30" s="39"/>
       <c r="E30" s="15"/>
@@ -3223,23 +3223,23 @@
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1">
       <c r="A31" s="36" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B31" s="37" t="s">
         <v>141</v>
       </c>
       <c r="C31" s="41" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E31" s="38" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="F31" s="18"/>
       <c r="G31" s="38" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
@@ -3264,19 +3264,19 @@
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
       <c r="A32" s="51" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B32" s="37" t="s">
         <v>141</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>142</v>
       </c>
       <c r="E32" s="38" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F32" s="9" t="s">
         <v>92</v>
@@ -3311,7 +3311,7 @@
         <v>141</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
@@ -3342,13 +3342,13 @@
     </row>
     <row r="34" spans="1:27" ht="15.75" customHeight="1">
       <c r="A34" s="25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B34" s="37" t="s">
         <v>25</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>174</v>
@@ -3381,13 +3381,13 @@
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1">
       <c r="A35" s="36" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B35" s="37" t="s">
         <v>25</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>146</v>
@@ -3426,7 +3426,7 @@
         <v>25</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>26</v>
@@ -3465,13 +3465,13 @@
         <v>25</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="E37" s="38" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F37" s="18" t="s">
         <v>177</v>
@@ -3506,13 +3506,13 @@
         <v>25</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="E38" s="38" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F38" s="30" t="s">
         <v>179</v>
@@ -3541,19 +3541,19 @@
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
       <c r="A39" s="26" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B39" s="37" t="s">
         <v>25</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D39" s="49" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E39" s="49" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F39" s="18"/>
       <c r="G39" s="29"/>
@@ -3586,13 +3586,13 @@
         <v>25</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="E40" s="38" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F40" s="18"/>
       <c r="G40" s="18"/>
@@ -3625,7 +3625,7 @@
         <v>25</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D41" s="10" t="s">
         <v>50</v>
@@ -3660,13 +3660,13 @@
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1">
       <c r="A42" s="24" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B42" s="37" t="s">
         <v>25</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>50</v>
@@ -3707,7 +3707,7 @@
         <v>25</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D43" s="18" t="s">
         <v>50</v>
@@ -3740,13 +3740,13 @@
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1">
       <c r="A44" s="25" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B44" s="37" t="s">
         <v>25</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>186</v>
@@ -3779,13 +3779,13 @@
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1">
       <c r="A45" s="36" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B45" s="37" t="s">
         <v>25</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>22</v>
@@ -3818,13 +3818,13 @@
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1">
       <c r="A46" s="36" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B46" s="37" t="s">
         <v>25</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>202</v>
@@ -3833,7 +3833,7 @@
         <v>200</v>
       </c>
       <c r="F46" s="38" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="G46" s="10"/>
       <c r="H46" s="8"/>
@@ -3859,13 +3859,13 @@
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1">
       <c r="A47" s="50" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B47" s="37" t="s">
         <v>25</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>190</v>
@@ -3904,7 +3904,7 @@
         <v>25</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D48" s="9" t="s">
         <v>105</v>
@@ -3939,13 +3939,13 @@
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1">
       <c r="A49" s="26" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B49" s="37" t="s">
         <v>25</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D49" s="18" t="s">
         <v>105</v>
@@ -3978,13 +3978,13 @@
     </row>
     <row r="50" spans="1:27" ht="15.75" customHeight="1">
       <c r="A50" s="50" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B50" s="37" t="s">
         <v>25</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>197</v>
@@ -4023,7 +4023,7 @@
         <v>25</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D51" s="18" t="s">
         <v>120</v>
@@ -4056,23 +4056,23 @@
     </row>
     <row r="52" spans="1:27" ht="15.75" customHeight="1">
       <c r="A52" s="36" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B52" s="37" t="s">
         <v>25</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="E52" s="38" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="F52" s="30"/>
       <c r="G52" s="63" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="H52" s="9"/>
       <c r="I52" s="9"/>
@@ -4103,7 +4103,7 @@
         <v>25</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D53" s="18" t="s">
         <v>117</v>
@@ -4136,19 +4136,19 @@
     </row>
     <row r="54" spans="1:27" ht="15.75" customHeight="1">
       <c r="A54" s="51" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B54" s="37" t="s">
         <v>25</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D54" s="38" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E54" s="38" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="F54" s="18"/>
       <c r="G54" s="18"/>
@@ -4175,18 +4175,18 @@
     </row>
     <row r="55" spans="1:27" ht="15.75" customHeight="1">
       <c r="A55" s="36" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B55" s="37" t="s">
         <v>25</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D55" s="38"/>
       <c r="E55" s="18"/>
       <c r="F55" s="18" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G55" s="18"/>
       <c r="H55" s="8"/>
@@ -4218,7 +4218,7 @@
         <v>25</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D56" s="18"/>
       <c r="E56" s="18"/>
@@ -4249,13 +4249,13 @@
     </row>
     <row r="57" spans="1:27" ht="15.75" customHeight="1">
       <c r="A57" s="24" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B57" s="37" t="s">
         <v>25</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D57" s="18"/>
       <c r="E57" s="18"/>
@@ -4292,7 +4292,7 @@
         <v>25</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D58" s="18"/>
       <c r="E58" s="18"/>
@@ -4329,7 +4329,7 @@
         <v>25</v>
       </c>
       <c r="C59" s="19" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D59" s="18"/>
       <c r="E59" s="18"/>
@@ -4358,13 +4358,13 @@
     </row>
     <row r="60" spans="1:27" ht="15.75" customHeight="1">
       <c r="A60" s="57" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B60" s="37" t="s">
         <v>25</v>
       </c>
       <c r="C60" s="19" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D60" s="18"/>
       <c r="E60" s="18"/>
@@ -4399,7 +4399,7 @@
         <v>25</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
@@ -4428,19 +4428,19 @@
     </row>
     <row r="62" spans="1:27" ht="15.75" customHeight="1">
       <c r="A62" s="51" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B62" s="37" t="s">
         <v>62</v>
       </c>
       <c r="C62" s="29" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D62" s="38" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="F62" s="30"/>
       <c r="G62" s="29"/>
@@ -4473,7 +4473,7 @@
         <v>62</v>
       </c>
       <c r="C63" s="19" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D63" s="18"/>
       <c r="E63" s="18"/>
@@ -4502,13 +4502,13 @@
     </row>
     <row r="64" spans="1:27" ht="15.75" customHeight="1">
       <c r="A64" s="36" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B64" s="37" t="s">
         <v>62</v>
       </c>
       <c r="C64" s="29" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D64" s="18"/>
       <c r="E64" s="18"/>
@@ -4537,13 +4537,13 @@
     </row>
     <row r="65" spans="1:27" ht="15.75" customHeight="1">
       <c r="A65" s="50" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B65" s="37" t="s">
         <v>89</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D65" s="18" t="s">
         <v>90</v>
@@ -4578,13 +4578,13 @@
     </row>
     <row r="66" spans="1:27" ht="15.75" customHeight="1">
       <c r="A66" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B66" s="37" t="s">
         <v>29</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D66" s="9" t="s">
         <v>174</v>
@@ -4623,7 +4623,7 @@
         <v>29</v>
       </c>
       <c r="C67" s="19" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D67" s="30" t="s">
         <v>26</v>
@@ -4662,13 +4662,13 @@
         <v>29</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D68" s="38" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E68" s="38" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F68" s="18"/>
       <c r="G68" s="18"/>
@@ -4701,13 +4701,13 @@
         <v>29</v>
       </c>
       <c r="C69" s="19" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D69" s="38" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="E69" s="38" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F69" s="18"/>
       <c r="G69" s="30"/>
@@ -4740,7 +4740,7 @@
         <v>29</v>
       </c>
       <c r="C70" s="19" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D70" s="18" t="s">
         <v>50</v>
@@ -4773,13 +4773,13 @@
     </row>
     <row r="71" spans="1:27" ht="15.75" customHeight="1">
       <c r="A71" s="54" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B71" s="37" t="s">
         <v>29</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D71" s="18" t="s">
         <v>50</v>
@@ -4818,7 +4818,7 @@
         <v>29</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D72" s="18" t="s">
         <v>60</v>
@@ -4851,13 +4851,13 @@
     </row>
     <row r="73" spans="1:27" ht="15.75" customHeight="1">
       <c r="A73" s="25" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B73" s="37" t="s">
         <v>29</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D73" s="9" t="s">
         <v>186</v>
@@ -4890,13 +4890,13 @@
     </row>
     <row r="74" spans="1:27" ht="15.75" customHeight="1">
       <c r="A74" s="24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B74" s="37" t="s">
         <v>29</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D74" s="9" t="s">
         <v>22</v>
@@ -4937,7 +4937,7 @@
         <v>29</v>
       </c>
       <c r="C75" s="19" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D75" s="18" t="s">
         <v>22</v>
@@ -4970,13 +4970,13 @@
     </row>
     <row r="76" spans="1:27" ht="15.75" customHeight="1">
       <c r="A76" s="54" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B76" s="37" t="s">
         <v>29</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D76" s="10" t="s">
         <v>22</v>
@@ -5009,13 +5009,13 @@
     </row>
     <row r="77" spans="1:27" ht="15.75" customHeight="1">
       <c r="A77" s="24" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B77" s="37" t="s">
         <v>29</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D77" s="9" t="s">
         <v>202</v>
@@ -5050,13 +5050,13 @@
     </row>
     <row r="78" spans="1:27" ht="15.75" customHeight="1">
       <c r="A78" s="50" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B78" s="37" t="s">
         <v>29</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D78" s="9" t="s">
         <v>190</v>
@@ -5089,13 +5089,13 @@
     </row>
     <row r="79" spans="1:27" ht="15.75" customHeight="1">
       <c r="A79" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B79" s="37" t="s">
         <v>29</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D79" s="9" t="s">
         <v>171</v>
@@ -5136,7 +5136,7 @@
         <v>29</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D80" s="9" t="s">
         <v>171</v>
@@ -5171,13 +5171,13 @@
     </row>
     <row r="81" spans="1:27" ht="15.75" customHeight="1">
       <c r="A81" s="36" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B81" s="37" t="s">
         <v>29</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D81" s="7" t="s">
         <v>105</v>
@@ -5186,7 +5186,7 @@
         <v>106</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G81" s="10"/>
       <c r="H81" s="8"/>
@@ -5212,13 +5212,13 @@
     </row>
     <row r="82" spans="1:27" ht="15.75" customHeight="1">
       <c r="A82" s="50" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B82" s="37" t="s">
         <v>29</v>
       </c>
       <c r="C82" s="19" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D82" s="22" t="s">
         <v>75</v>
@@ -5257,7 +5257,7 @@
         <v>29</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D83" s="18" t="s">
         <v>181</v>
@@ -5290,18 +5290,18 @@
     </row>
     <row r="84" spans="1:27" ht="15.75" customHeight="1">
       <c r="A84" s="36" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B84" s="37" t="s">
         <v>29</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D84" s="18"/>
       <c r="E84" s="7"/>
       <c r="F84" s="7" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G84" s="10"/>
       <c r="H84" s="8"/>
@@ -5333,7 +5333,7 @@
         <v>29</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D85" s="9"/>
       <c r="E85" s="9"/>
@@ -5370,7 +5370,7 @@
         <v>29</v>
       </c>
       <c r="C86" s="19" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D86" s="30"/>
       <c r="E86" s="18"/>
@@ -5401,13 +5401,13 @@
     </row>
     <row r="87" spans="1:27" ht="15.75" customHeight="1">
       <c r="A87" s="59" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B87" s="37" t="s">
         <v>29</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D87" s="10"/>
       <c r="E87" s="7"/>
@@ -5444,7 +5444,7 @@
         <v>29</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D88" s="10"/>
       <c r="E88" s="10"/>
@@ -5473,13 +5473,13 @@
     </row>
     <row r="89" spans="1:27" ht="21" customHeight="1">
       <c r="A89" s="61" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B89" s="37" t="s">
         <v>29</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D89" s="10"/>
       <c r="E89" s="10"/>
@@ -5514,7 +5514,7 @@
         <v>29</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D90" s="9"/>
       <c r="E90" s="9"/>
@@ -5549,7 +5549,7 @@
         <v>45</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D91" s="10"/>
       <c r="E91" s="18"/>
@@ -5578,13 +5578,13 @@
     </row>
     <row r="92" spans="1:27" ht="15.75" customHeight="1">
       <c r="A92" s="40" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B92" s="37" t="s">
         <v>45</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D92" s="10"/>
       <c r="E92" s="10"/>
@@ -5619,7 +5619,7 @@
         <v>73</v>
       </c>
       <c r="C93" s="19" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D93" s="31"/>
       <c r="E93" s="31"/>
@@ -5648,13 +5648,13 @@
     </row>
     <row r="94" spans="1:27" ht="15.75" customHeight="1">
       <c r="A94" s="53" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B94" s="37" t="s">
         <v>74</v>
       </c>
       <c r="C94" s="19" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D94" s="18"/>
       <c r="E94" s="18"/>
@@ -5683,19 +5683,19 @@
     </row>
     <row r="95" spans="1:27" ht="15.75" customHeight="1">
       <c r="A95" s="55" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B95" s="37" t="s">
         <v>88</v>
       </c>
       <c r="C95" s="19" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D95" s="38" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E95" s="38" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="F95" s="30"/>
       <c r="G95" s="31"/>
@@ -5728,7 +5728,7 @@
         <v>88</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D96" s="7"/>
       <c r="E96" s="7"/>
@@ -5757,23 +5757,23 @@
     </row>
     <row r="97" spans="1:27" ht="15.75" customHeight="1">
       <c r="A97" s="36" t="s">
+        <v>296</v>
+      </c>
+      <c r="B97" s="37" t="s">
+        <v>297</v>
+      </c>
+      <c r="C97" s="19" t="s">
+        <v>394</v>
+      </c>
+      <c r="D97" s="38" t="s">
         <v>298</v>
       </c>
-      <c r="B97" s="37" t="s">
-        <v>299</v>
-      </c>
-      <c r="C97" s="19" t="s">
-        <v>397</v>
-      </c>
-      <c r="D97" s="38" t="s">
-        <v>300</v>
-      </c>
       <c r="E97" s="38" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="F97" s="18"/>
       <c r="G97" s="63" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H97" s="9"/>
       <c r="I97" s="9"/>
@@ -5804,7 +5804,7 @@
         <v>10</v>
       </c>
       <c r="C98" s="19" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D98" s="18" t="s">
         <v>30</v>
@@ -5841,13 +5841,13 @@
     </row>
     <row r="99" spans="1:27" ht="15.75" customHeight="1">
       <c r="A99" s="26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B99" s="37" t="s">
         <v>10</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D99" s="7" t="s">
         <v>30</v>
@@ -5888,7 +5888,7 @@
         <v>10</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D100" s="7" t="s">
         <v>94</v>
@@ -5929,7 +5929,7 @@
         <v>10</v>
       </c>
       <c r="C101" s="19" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D101" s="18" t="s">
         <v>108</v>
@@ -5968,7 +5968,7 @@
         <v>10</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D102" s="9"/>
       <c r="E102" s="18"/>
@@ -6003,7 +6003,7 @@
         <v>129</v>
       </c>
       <c r="C103" s="19" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D103" s="18" t="s">
         <v>132</v>
@@ -6042,7 +6042,7 @@
         <v>129</v>
       </c>
       <c r="C104" s="19" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D104" s="18" t="s">
         <v>134</v>
@@ -6081,7 +6081,7 @@
         <v>46</v>
       </c>
       <c r="C105" s="19" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D105" s="18"/>
       <c r="E105" s="18"/>
@@ -6116,7 +6116,7 @@
         <v>100</v>
       </c>
       <c r="C106" s="19" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D106" s="18"/>
       <c r="E106" s="18"/>
@@ -6145,13 +6145,13 @@
     </row>
     <row r="107" spans="1:27" ht="15.75" customHeight="1">
       <c r="A107" s="16" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B107" s="37" t="s">
         <v>101</v>
       </c>
       <c r="C107" s="19" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="D107" s="18" t="s">
         <v>22</v>
@@ -6190,7 +6190,7 @@
         <v>101</v>
       </c>
       <c r="C108" s="19" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="D108" s="18"/>
       <c r="E108" s="18"/>
@@ -6225,7 +6225,7 @@
         <v>102</v>
       </c>
       <c r="C109" s="19" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D109" s="18"/>
       <c r="E109" s="18"/>
@@ -6260,7 +6260,7 @@
         <v>111</v>
       </c>
       <c r="C110" s="19" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D110" s="18" t="s">
         <v>112</v>
@@ -6301,7 +6301,7 @@
         <v>124</v>
       </c>
       <c r="C111" s="19" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D111" s="18"/>
       <c r="E111" s="18"/>
@@ -6332,19 +6332,19 @@
     </row>
     <row r="112" spans="1:27" ht="15.75" customHeight="1">
       <c r="A112" s="36" t="s">
-        <v>316</v>
+        <v>455</v>
       </c>
       <c r="B112" s="37" t="s">
         <v>16</v>
       </c>
       <c r="C112" s="19" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D112" s="38" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E112" s="38" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="F112" s="18"/>
       <c r="G112" s="18"/>
@@ -6371,13 +6371,13 @@
     </row>
     <row r="113" spans="1:27" ht="15.75" customHeight="1">
       <c r="A113" s="50" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B113" s="37" t="s">
         <v>16</v>
       </c>
       <c r="C113" s="19" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D113" s="18" t="s">
         <v>53</v>
@@ -6416,7 +6416,7 @@
         <v>16</v>
       </c>
       <c r="C114" s="19" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D114" s="30" t="s">
         <v>78</v>
@@ -6455,7 +6455,7 @@
         <v>16</v>
       </c>
       <c r="C115" s="19" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D115" s="31" t="s">
         <v>84</v>
@@ -6488,22 +6488,22 @@
     </row>
     <row r="116" spans="1:27" ht="15.75" customHeight="1">
       <c r="A116" s="36" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B116" s="37" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C116" s="41" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D116" s="38" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="E116" s="38" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="F116" s="29" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G116" s="29"/>
       <c r="H116" s="8"/>
@@ -6529,22 +6529,22 @@
     </row>
     <row r="117" spans="1:27" ht="15.75" customHeight="1">
       <c r="A117" s="36" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B117" s="37" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C117" s="41" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D117" s="38" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="E117" s="38" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="F117" s="29" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G117" s="37"/>
       <c r="H117" s="8"/>
@@ -6576,7 +6576,7 @@
         <v>116</v>
       </c>
       <c r="C118" s="19" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D118" s="18"/>
       <c r="E118" s="18"/>
@@ -6613,13 +6613,13 @@
         <v>116</v>
       </c>
       <c r="C119" s="19" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D119" s="18"/>
       <c r="E119" s="18"/>
       <c r="F119" s="18"/>
       <c r="G119" s="29" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H119" s="9"/>
       <c r="I119" s="9"/>
@@ -6650,13 +6650,13 @@
         <v>18</v>
       </c>
       <c r="C120" s="19" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D120" s="18" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="E120" s="38" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="F120" s="18"/>
       <c r="G120" s="30"/>
@@ -6689,7 +6689,7 @@
         <v>128</v>
       </c>
       <c r="C121" s="19" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D121" s="18"/>
       <c r="E121" s="18"/>
@@ -6726,7 +6726,7 @@
         <v>138</v>
       </c>
       <c r="C122" s="19" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D122" s="18"/>
       <c r="E122" s="18"/>
@@ -6761,7 +6761,7 @@
         <v>139</v>
       </c>
       <c r="C123" s="19" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D123" s="18"/>
       <c r="E123" s="18"/>
@@ -6790,13 +6790,13 @@
     </row>
     <row r="124" spans="1:27" ht="15.75" customHeight="1">
       <c r="A124" s="50" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B124" s="37" t="s">
         <v>55</v>
       </c>
       <c r="C124" s="19" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D124" s="18" t="s">
         <v>53</v>
@@ -6837,7 +6837,7 @@
         <v>55</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D125" s="18"/>
       <c r="E125" s="18"/>
@@ -6866,19 +6866,19 @@
     </row>
     <row r="126" spans="1:27" ht="15.75" customHeight="1">
       <c r="A126" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B126" s="37" t="s">
         <v>65</v>
       </c>
       <c r="C126" s="19" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D126" s="64" t="s">
         <v>205</v>
       </c>
       <c r="E126" s="18" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="F126" s="18" t="s">
         <v>206</v>
@@ -6907,19 +6907,19 @@
     </row>
     <row r="127" spans="1:27" ht="15.75" customHeight="1">
       <c r="A127" s="33" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B127" s="37" t="s">
         <v>65</v>
       </c>
       <c r="C127" s="19" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D127" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E127" s="18" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="F127" s="18"/>
       <c r="G127" s="18"/>
@@ -6952,7 +6952,7 @@
         <v>65</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D128" s="18" t="s">
         <v>66</v>
@@ -6991,7 +6991,7 @@
         <v>65</v>
       </c>
       <c r="C129" s="19" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D129" s="30" t="s">
         <v>80</v>
@@ -7024,13 +7024,13 @@
     </row>
     <row r="130" spans="1:27" ht="15.75" customHeight="1">
       <c r="A130" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B130" s="37" t="s">
         <v>65</v>
       </c>
       <c r="C130" s="19" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D130" s="18" t="s">
         <v>80</v>
@@ -7063,19 +7063,19 @@
     </row>
     <row r="131" spans="1:27" ht="15.75" customHeight="1">
       <c r="A131" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B131" s="37" t="s">
         <v>65</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D131" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E131" s="21" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="F131" s="7" t="s">
         <v>206</v>
@@ -7104,19 +7104,19 @@
     </row>
     <row r="132" spans="1:27" ht="15.75" customHeight="1">
       <c r="A132" s="23" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B132" s="37" t="s">
         <v>65</v>
       </c>
       <c r="C132" s="19" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D132" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E132" s="21" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="F132" s="7" t="s">
         <v>206</v>
@@ -7151,7 +7151,7 @@
         <v>65</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D133" s="30"/>
       <c r="E133" s="7"/>
@@ -7186,7 +7186,7 @@
         <v>65</v>
       </c>
       <c r="C134" s="19" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D134" s="18"/>
       <c r="E134" s="18"/>
@@ -7215,19 +7215,19 @@
     </row>
     <row r="135" spans="1:27" ht="15.75" customHeight="1">
       <c r="A135" s="33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B135" s="37" t="s">
         <v>150</v>
       </c>
       <c r="C135" s="65" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D135" s="38" t="s">
         <v>207</v>
       </c>
       <c r="E135" s="10" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="F135" s="7"/>
       <c r="G135" s="10"/>
@@ -7254,16 +7254,16 @@
     </row>
     <row r="136" spans="1:27" ht="15.75" customHeight="1">
       <c r="A136" s="23" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B136" s="37" t="s">
         <v>150</v>
       </c>
       <c r="C136" s="65" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D136" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E136" s="17" t="s">
         <v>81</v>
@@ -7293,16 +7293,16 @@
     </row>
     <row r="137" spans="1:27" ht="15.75" customHeight="1">
       <c r="A137" s="33" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B137" s="37" t="s">
         <v>150</v>
       </c>
       <c r="C137" s="65" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D137" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E137" s="17" t="s">
         <v>81</v>
@@ -7332,19 +7332,19 @@
     </row>
     <row r="138" spans="1:27" ht="18.75" customHeight="1">
       <c r="A138" s="47" t="s">
-        <v>211</v>
+        <v>453</v>
       </c>
       <c r="B138" s="37" t="s">
         <v>87</v>
       </c>
       <c r="C138" s="41" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D138" s="38" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="E138" s="38" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="F138" s="38" t="s">
         <v>114</v>
@@ -7373,13 +7373,13 @@
     </row>
     <row r="139" spans="1:27" ht="15.75" customHeight="1">
       <c r="A139" s="36" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B139" s="37" t="s">
         <v>87</v>
       </c>
       <c r="C139" s="41" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D139" s="10" t="s">
         <v>50</v>
@@ -7418,7 +7418,7 @@
         <v>87</v>
       </c>
       <c r="C140" s="41" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D140" s="10" t="s">
         <v>80</v>
@@ -7451,13 +7451,13 @@
     </row>
     <row r="141" spans="1:27" ht="15.75" customHeight="1">
       <c r="A141" s="25" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B141" s="37" t="s">
         <v>87</v>
       </c>
       <c r="C141" s="41" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D141" s="10" t="s">
         <v>80</v>
@@ -7496,7 +7496,7 @@
         <v>151</v>
       </c>
       <c r="C142" s="41" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D142" s="10"/>
       <c r="E142" s="10"/>
@@ -7531,7 +7531,7 @@
         <v>7</v>
       </c>
       <c r="C143" s="41" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D143" s="37" t="s">
         <v>155</v>
@@ -7572,13 +7572,13 @@
         <v>7</v>
       </c>
       <c r="C144" s="41" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D144" s="44" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E144" s="38" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="F144" s="7" t="s">
         <v>156</v>
@@ -7607,19 +7607,19 @@
     </row>
     <row r="145" spans="1:27" ht="15.75" customHeight="1">
       <c r="A145" s="48" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B145" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C145" s="41" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D145" s="46" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E145" s="38" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="F145" s="7" t="s">
         <v>156</v>
@@ -7654,13 +7654,13 @@
         <v>7</v>
       </c>
       <c r="C146" s="41" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D146" s="46" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="E146" s="46" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="F146" s="7" t="s">
         <v>156</v>
@@ -7695,13 +7695,13 @@
         <v>7</v>
       </c>
       <c r="C147" s="41" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D147" s="18" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E147" s="18" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F147" s="18"/>
       <c r="G147" s="18"/>
@@ -7734,13 +7734,13 @@
         <v>7</v>
       </c>
       <c r="C148" s="41" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D148" s="10" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="E148" s="10" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F148" s="7"/>
       <c r="G148" s="10"/>
@@ -7767,19 +7767,19 @@
     </row>
     <row r="149" spans="1:27" ht="15.75" customHeight="1">
       <c r="A149" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B149" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C149" s="41" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D149" s="29" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="E149" s="29" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="F149" s="7"/>
       <c r="G149" s="29"/>
@@ -7806,19 +7806,19 @@
     </row>
     <row r="150" spans="1:27" ht="15.75" customHeight="1">
       <c r="A150" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B150" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C150" s="9" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D150" s="29" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E150" s="9" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="F150" s="9"/>
       <c r="G150" s="29"/>
@@ -7845,19 +7845,19 @@
     </row>
     <row r="151" spans="1:27" ht="15.75" customHeight="1">
       <c r="A151" s="33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B151" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C151" s="41" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D151" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="E151" s="18" t="s">
         <v>213</v>
-      </c>
-      <c r="E151" s="18" t="s">
-        <v>214</v>
       </c>
       <c r="F151" s="7"/>
       <c r="G151" s="10"/>
@@ -7884,19 +7884,19 @@
     </row>
     <row r="152" spans="1:27" ht="15.75" customHeight="1">
       <c r="A152" s="23" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B152" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C152" s="41" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D152" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="E152" s="30" t="s">
         <v>213</v>
-      </c>
-      <c r="E152" s="30" t="s">
-        <v>214</v>
       </c>
       <c r="F152" s="7"/>
       <c r="G152" s="30"/>
@@ -7923,19 +7923,19 @@
     </row>
     <row r="153" spans="1:27" ht="15.75" customHeight="1">
       <c r="A153" s="35" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B153" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D153" s="15" t="s">
         <v>164</v>
       </c>
       <c r="E153" s="15" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F153" s="7"/>
       <c r="G153" s="29"/>
@@ -7968,7 +7968,7 @@
         <v>7</v>
       </c>
       <c r="C154" s="66" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D154" s="10" t="s">
         <v>69</v>
@@ -8001,19 +8001,19 @@
     </row>
     <row r="155" spans="1:27" ht="21" customHeight="1">
       <c r="A155" s="23" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B155" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C155" s="66" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D155" s="18" t="s">
         <v>8</v>
       </c>
       <c r="E155" s="10" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F155" s="7"/>
       <c r="G155" s="37"/>
@@ -8040,19 +8040,19 @@
     </row>
     <row r="156" spans="1:27" ht="15.75" customHeight="1">
       <c r="A156" s="23" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B156" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C156" s="41" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D156" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E156" s="10" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F156" s="7"/>
       <c r="G156" s="29"/>
@@ -8079,19 +8079,19 @@
     </row>
     <row r="157" spans="1:27" ht="15.75" customHeight="1">
       <c r="A157" s="23" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B157" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C157" s="41" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D157" s="18" t="s">
         <v>8</v>
       </c>
       <c r="E157" s="18" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F157" s="7"/>
       <c r="G157" s="29"/>
@@ -8118,16 +8118,16 @@
     </row>
     <row r="158" spans="1:27" ht="15.75" customHeight="1">
       <c r="A158" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B158" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C158" s="41" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D158" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E158" s="18" t="s">
         <v>70</v>
@@ -8157,16 +8157,16 @@
     </row>
     <row r="159" spans="1:27" ht="15.75" customHeight="1">
       <c r="A159" s="23" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B159" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C159" s="41" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D159" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E159" s="18" t="s">
         <v>70</v>
@@ -8196,16 +8196,16 @@
     </row>
     <row r="160" spans="1:27" ht="15.75" customHeight="1">
       <c r="A160" s="23" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B160" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C160" s="41" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D160" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E160" s="10" t="s">
         <v>70</v>
@@ -8235,25 +8235,25 @@
     </row>
     <row r="161" spans="1:27" ht="30.75" customHeight="1">
       <c r="A161" s="36" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B161" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C161" s="41" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D161" s="38" t="s">
         <v>163</v>
       </c>
       <c r="E161" s="38" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="F161" s="38" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G161" s="38" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="H161" s="8"/>
       <c r="I161" s="8"/>
@@ -8278,13 +8278,13 @@
     </row>
     <row r="162" spans="1:27" ht="15.75" customHeight="1">
       <c r="A162" s="34" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B162" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C162" s="38" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D162" s="18" t="s">
         <v>22</v>
@@ -8323,7 +8323,7 @@
         <v>7</v>
       </c>
       <c r="C163" s="41" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D163" s="29" t="s">
         <v>158</v>
@@ -8358,13 +8358,13 @@
     </row>
     <row r="164" spans="1:27" ht="15.75" customHeight="1">
       <c r="A164" s="34" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B164" s="68" t="s">
         <v>7</v>
       </c>
       <c r="C164" s="41" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D164" s="18"/>
       <c r="E164" s="10"/>
@@ -8399,7 +8399,7 @@
         <v>7</v>
       </c>
       <c r="C165" s="41" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D165" s="18"/>
       <c r="E165" s="18"/>
@@ -8434,7 +8434,7 @@
         <v>7</v>
       </c>
       <c r="C166" s="67" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D166" s="9"/>
       <c r="E166" s="9"/>
@@ -8469,7 +8469,7 @@
         <v>152</v>
       </c>
       <c r="C167" s="41" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D167" s="30"/>
       <c r="E167" s="18"/>
@@ -8504,16 +8504,16 @@
         <v>7</v>
       </c>
       <c r="C168" s="67" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D168" s="38" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E168" s="38" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F168" s="7" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="G168" s="10"/>
       <c r="H168" s="8"/>
@@ -8545,7 +8545,7 @@
         <v>168</v>
       </c>
       <c r="C169" s="41" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D169" s="18"/>
       <c r="E169" s="18"/>
@@ -8574,13 +8574,13 @@
     </row>
     <row r="170" spans="1:27" ht="15.75" customHeight="1">
       <c r="A170" s="11" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B170" s="37" t="s">
         <v>168</v>
       </c>
       <c r="C170" s="41" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D170" s="18"/>
       <c r="E170" s="18"/>
@@ -8609,19 +8609,19 @@
     </row>
     <row r="171" spans="1:27" ht="15.75" customHeight="1">
       <c r="A171" s="36" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B171" s="37" t="s">
         <v>41</v>
       </c>
       <c r="C171" s="41" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D171" s="38" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E171" s="38" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="F171" s="7"/>
       <c r="G171" s="10"/>
@@ -8654,7 +8654,7 @@
         <v>41</v>
       </c>
       <c r="C172" s="41" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D172" s="10" t="s">
         <v>42</v>
@@ -8687,19 +8687,19 @@
     </row>
     <row r="173" spans="1:27" ht="15.75" customHeight="1">
       <c r="A173" s="40" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B173" s="37" t="s">
         <v>41</v>
       </c>
       <c r="C173" s="41" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D173" s="38" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E173" s="38" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F173" s="7"/>
       <c r="G173" s="10"/>
@@ -8732,10 +8732,10 @@
         <v>41</v>
       </c>
       <c r="C174" s="41" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D174" s="18" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="E174" s="38" t="s">
         <v>48</v>
@@ -8771,7 +8771,7 @@
         <v>41</v>
       </c>
       <c r="C175" s="41" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D175" s="18"/>
       <c r="E175" s="18"/>
@@ -8800,13 +8800,13 @@
     </row>
     <row r="176" spans="1:27" ht="15.75" customHeight="1">
       <c r="A176" s="36" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B176" s="37" t="s">
         <v>169</v>
       </c>
       <c r="C176" s="41" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D176" s="38" t="s">
         <v>66</v>
@@ -8814,7 +8814,7 @@
       <c r="E176" s="18"/>
       <c r="F176" s="7"/>
       <c r="G176" s="38" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H176" s="8"/>
       <c r="I176" s="8"/>
@@ -8839,19 +8839,19 @@
     </row>
     <row r="177" spans="1:27" ht="15.75" customHeight="1">
       <c r="A177" s="33" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B177" s="37" t="s">
         <v>169</v>
       </c>
       <c r="C177" s="41" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D177" s="29" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E177" s="18" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="F177" s="18"/>
       <c r="G177" s="10"/>
@@ -8878,19 +8878,19 @@
     </row>
     <row r="178" spans="1:27" ht="15.75" customHeight="1">
       <c r="A178" s="36" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B178" s="37" t="s">
         <v>169</v>
       </c>
       <c r="C178" s="41" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D178" s="62" t="s">
         <v>80</v>
       </c>
       <c r="E178" s="38" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="F178" s="18"/>
       <c r="G178" s="18"/>
@@ -8923,7 +8923,7 @@
         <v>169</v>
       </c>
       <c r="C179" s="41" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D179" s="18"/>
       <c r="E179" s="18"/>
@@ -8952,19 +8952,19 @@
     </row>
     <row r="180" spans="1:27" ht="15.75" customHeight="1">
       <c r="A180" s="36" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B180" s="37" t="s">
         <v>196</v>
       </c>
       <c r="C180" s="41" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D180" s="38" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E180" s="38" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="F180" s="30"/>
       <c r="G180" s="30"/>
@@ -8997,7 +8997,7 @@
         <v>137</v>
       </c>
       <c r="C181" s="41" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D181" s="18" t="s">
         <v>105</v>
@@ -9030,13 +9030,13 @@
     </row>
     <row r="182" spans="1:27" ht="15.75" customHeight="1">
       <c r="A182" s="36" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B182" s="37" t="s">
         <v>137</v>
       </c>
       <c r="C182" s="41" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D182" s="18" t="s">
         <v>105</v>
@@ -9075,7 +9075,7 @@
         <v>137</v>
       </c>
       <c r="C183" s="41" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D183" s="18"/>
       <c r="E183" s="18"/>
@@ -9104,19 +9104,19 @@
     </row>
     <row r="184" spans="1:27" ht="15.75" customHeight="1">
       <c r="A184" s="23" t="s">
-        <v>236</v>
+        <v>454</v>
       </c>
       <c r="B184" s="37" t="s">
         <v>195</v>
       </c>
       <c r="C184" s="41" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="D184" s="38" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="E184" s="38" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="F184" s="18"/>
       <c r="G184" s="10"/>
@@ -9143,13 +9143,13 @@
     </row>
     <row r="185" spans="1:27" ht="15.75" customHeight="1">
       <c r="A185" s="36" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B185" s="37" t="s">
         <v>195</v>
       </c>
       <c r="C185" s="41" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="D185" s="18" t="s">
         <v>50</v>

</xml_diff>